<commit_message>
Datasets changes and Modification
</commit_message>
<xml_diff>
--- a/Decider OM Resources/dataset2/decider_authentic_datasets_no_space.xlsx
+++ b/Decider OM Resources/dataset2/decider_authentic_datasets_no_space.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/Decider OM Resources/dataset2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BCA0CD-B1A1-AD46-BB5C-40607A20A0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4D1F5C-DCCC-A940-B79D-5586E3815F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{4B5CD0E9-7389-934A-B8F8-5EA3DA903C2F}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{4B5CD0E9-7389-934A-B8F8-5EA3DA903C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -852,12 +852,12 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="151.5" customWidth="1"/>
+    <col min="1" max="1" width="122" customWidth="1"/>
     <col min="2" max="2" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>